<commit_message>
add review sheet for assignment 02
</commit_message>
<xml_diff>
--- a/reviewsheet/review_points_kaungkhantnaing.xlsx
+++ b/reviewsheet/review_points_kaungkhantnaing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KaungKhantNaing\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975E9CC6-E568-45C8-978E-B536223F0A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A95F8B-3A5B-4866-90D7-BD7CE3428EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Head" sheetId="1" r:id="rId1"/>
@@ -22,19 +22,27 @@
     <sheet name="Sample Task List" sheetId="8" r:id="rId7"/>
     <sheet name="Task List with SCM Frame" sheetId="9" r:id="rId8"/>
     <sheet name="Assignment01" sheetId="10" r:id="rId9"/>
-    <sheet name="Ref." sheetId="3" r:id="rId10"/>
+    <sheet name="Assignment02" sheetId="12" r:id="rId10"/>
+    <sheet name="Ref." sheetId="3" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="133">
   <si>
     <t>Open</t>
     <phoneticPr fontId="1"/>
@@ -476,6 +484,33 @@
   </si>
   <si>
     <t>add params</t>
+  </si>
+  <si>
+    <t>Kaung Khant Naing</t>
+  </si>
+  <si>
+    <t>1) show file name</t>
+  </si>
+  <si>
+    <t>UX improvement</t>
+  </si>
+  <si>
+    <t>1) show success message after import 2) show list of imported data</t>
+  </si>
+  <si>
+    <t>1) type submit button</t>
+  </si>
+  <si>
+    <t>submite type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed and added </t>
+  </si>
+  <si>
+    <t>add success message and upload failed message</t>
+  </si>
+  <si>
+    <t>add type="submit" attribute in button</t>
   </si>
 </sst>
 </file>
@@ -675,7 +710,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -754,6 +789,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -786,6 +824,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1910,6 +1969,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>179916</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>412750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>95678</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1050845</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32E43329-B669-4D76-BBF7-7A8D7211280F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6074833" y="836083"/>
+          <a:ext cx="5038095" cy="638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63499</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>349251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>624416</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>598055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75821F48-A9A9-4C42-9F98-E962E2EA23C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5958416" y="2317751"/>
+          <a:ext cx="4000500" cy="248804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -2638,11 +2790,278 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBB6DA5-C5EB-40B6-9E2E-F62F26A923B1}">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:U4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.5" style="15" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="15" customWidth="1"/>
+    <col min="6" max="14" width="9" style="15"/>
+    <col min="15" max="15" width="13" style="15" customWidth="1"/>
+    <col min="16" max="21" width="9" style="15"/>
+    <col min="22" max="22" width="14.625" style="15" customWidth="1"/>
+    <col min="23" max="23" width="12.5" style="15" customWidth="1"/>
+    <col min="24" max="24" width="32.5" style="15" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="33" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="96" customHeight="1">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20">
+        <v>44494</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="38"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="44">
+        <v>44207</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="X2" s="18"/>
+    </row>
+    <row r="3" spans="1:24" ht="25.5" customHeight="1">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20">
+        <v>44494</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="44">
+        <v>44207</v>
+      </c>
+      <c r="W3" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="X3" s="18"/>
+    </row>
+    <row r="4" spans="1:24" ht="57" customHeight="1">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20">
+        <v>44494</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="44">
+        <v>44207</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="X4" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="P4:U4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FFA9095A-E3FD-448E-9E33-BDAC5C3B1D29}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D5E55C52-C9D8-4551-8C33-AFD1B70A4727}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$E$2:$E$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2:W4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C044DE1-8217-4519-B52C-0811E90EA5A8}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$D$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{772C9C2D-DC04-43BE-A110-9841097707D4}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$C$2:$C$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E3A5651A-2596-4565-ADA9-43DCC819B7B3}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2747,7 +3166,9 @@
         <v>29</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="10"/>
@@ -2866,30 +3287,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -2916,28 +3337,28 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>82</v>
       </c>
@@ -2962,28 +3383,28 @@
       <c r="E3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
       <c r="V3" s="18" t="s">
         <v>82</v>
       </c>
@@ -3008,33 +3429,33 @@
       <c r="E4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27" t="s">
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
       <c r="V4" s="18" t="s">
         <v>82</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X4" s="18"/>
     </row>
@@ -3100,8 +3521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13264516-45EC-4B12-9C49-DDC008555DF7}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="C2" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView view="pageBreakPreview" topLeftCell="H4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3136,30 +3557,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -3186,33 +3607,33 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>73</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X2" s="18"/>
     </row>
@@ -3232,33 +3653,33 @@
       <c r="E3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
       <c r="V3" s="18" t="s">
         <v>73</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X3" s="18"/>
     </row>
@@ -3278,33 +3699,33 @@
       <c r="E4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27" t="s">
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
       <c r="V4" s="18" t="s">
         <v>73</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X4" s="18"/>
     </row>
@@ -3369,7 +3790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5105948C-7804-4434-B607-79DA3F85CE6C}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="H1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
@@ -3405,30 +3826,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -3455,33 +3876,33 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>73</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X2" s="18"/>
     </row>
@@ -3541,7 +3962,7 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="M1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3576,30 +3997,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -3626,33 +4047,33 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>73</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X2" s="18"/>
     </row>
@@ -3672,33 +4093,33 @@
       <c r="E3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
       <c r="V3" s="18" t="s">
         <v>73</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X3" s="18"/>
     </row>
@@ -3761,8 +4182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017E22DB-897C-4CBD-B355-A546CADAE648}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="C1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3797,30 +4218,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -3847,31 +4268,31 @@
       <c r="E2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>66</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X2" s="18" t="s">
         <v>68</v>
@@ -3893,31 +4314,31 @@
       <c r="E3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
       <c r="V3" s="18" t="s">
         <v>66</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X3" s="18"/>
     </row>
@@ -3937,33 +4358,33 @@
       <c r="E4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27" t="s">
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
       <c r="V4" s="18" t="s">
         <v>66</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X4" s="18"/>
     </row>
@@ -3983,31 +4404,31 @@
       <c r="E5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="30" t="s">
+      <c r="P5" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="30"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
       <c r="V5" s="18" t="s">
         <v>66</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X5" s="18"/>
     </row>
@@ -4075,8 +4496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A935C436-83B6-4944-84D7-100E4F279E3B}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="D1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView view="pageBreakPreview" topLeftCell="L1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4111,30 +4532,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
       <c r="V1" s="17" t="s">
         <v>60</v>
       </c>
@@ -4161,33 +4582,33 @@
       <c r="E2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X2" s="18"/>
     </row>
@@ -4246,8 +4667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79EE276-69FB-47B7-AEE4-B8429CEE434E}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7:U7"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4282,30 +4703,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -4332,33 +4753,33 @@
       <c r="E2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>86</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X2" s="18"/>
     </row>
@@ -4378,31 +4799,31 @@
       <c r="E3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
       <c r="V3" s="18" t="s">
         <v>86</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X3" s="18"/>
     </row>
@@ -4422,31 +4843,31 @@
       <c r="E4" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
       <c r="V4" s="18" t="s">
         <v>86</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X4" s="18"/>
     </row>
@@ -4466,31 +4887,31 @@
       <c r="E5" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="30" t="s">
+      <c r="P5" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="30"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
       <c r="V5" s="18" t="s">
         <v>86</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X5" s="18"/>
     </row>
@@ -4510,26 +4931,26 @@
       <c r="E6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27" t="s">
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="30" t="s">
+      <c r="P6" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
       <c r="V6" s="18" t="s">
         <v>86</v>
       </c>
@@ -4552,31 +4973,31 @@
       <c r="E7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27" t="s">
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="30"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="30" t="s">
+      <c r="P7" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
       <c r="V7" s="18" t="s">
         <v>86</v>
       </c>
       <c r="W7" s="18" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="X7" s="18"/>
     </row>
@@ -4613,8 +5034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394B31C0-9FA0-4662-B312-DAF429ECDB72}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="L4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6:U6"/>
+    <sheetView view="pageBreakPreview" topLeftCell="L1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4649,30 +5070,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
       <c r="V1" s="17" t="s">
         <v>60</v>
       </c>
@@ -4699,31 +5120,31 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X2" s="18"/>
     </row>
@@ -4743,33 +5164,33 @@
       <c r="E3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
       <c r="V3" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X3" s="18"/>
     </row>
@@ -4789,33 +5210,33 @@
       <c r="E4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27" t="s">
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
       <c r="V4" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X4" s="18"/>
     </row>
@@ -4835,33 +5256,33 @@
       <c r="E5" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27" t="s">
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="30" t="s">
+      <c r="P5" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="30"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
       <c r="V5" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X5" s="18"/>
     </row>
@@ -4881,33 +5302,33 @@
       <c r="E6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27" t="s">
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="30" t="s">
+      <c r="P6" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
       <c r="V6" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W6" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X6" s="18"/>
     </row>
@@ -4927,33 +5348,33 @@
       <c r="E7" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27" t="s">
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="30"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="30" t="s">
+      <c r="P7" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
       <c r="V7" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W7" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X7" s="18"/>
     </row>
@@ -4973,33 +5394,33 @@
       <c r="E8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27" t="s">
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="30"/>
       <c r="O8" s="16"/>
-      <c r="P8" s="30" t="s">
+      <c r="P8" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="30"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
       <c r="V8" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W8" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X8" s="18"/>
     </row>
@@ -5019,31 +5440,31 @@
       <c r="E9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27" t="s">
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="30"/>
       <c r="O9" s="16"/>
-      <c r="P9" s="30" t="s">
+      <c r="P9" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
       <c r="V9" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W9" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X9" s="18"/>
     </row>
@@ -5063,33 +5484,33 @@
       <c r="E10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="27" t="s">
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="30"/>
       <c r="O10" s="16"/>
-      <c r="P10" s="30" t="s">
+      <c r="P10" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
       <c r="V10" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W10" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X10" s="18"/>
     </row>
@@ -5109,31 +5530,31 @@
       <c r="E11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="27" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="30"/>
       <c r="O11" s="16"/>
-      <c r="P11" s="30" t="s">
+      <c r="P11" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
       <c r="V11" s="18" t="s">
         <v>64</v>
       </c>
       <c r="W11" s="18" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="X11" s="18"/>
     </row>
@@ -5178,7 +5599,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1B399EE9-1C37-4054-8D1B-EB08957349CA}">
           <x14:formula1>
             <xm:f>'Ref.'!$A$2:$A$4</xm:f>

</xml_diff>

<commit_message>
add assignment 03 review fixed
</commit_message>
<xml_diff>
--- a/reviewsheet/review_points_kaungkhantnaing.xlsx
+++ b/reviewsheet/review_points_kaungkhantnaing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KaungKhantNaing\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\php_training\reviewsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A95F8B-3A5B-4866-90D7-BD7CE3428EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB0717C-7CF6-4BEF-BAF3-D3058BD76DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Head" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="Task List with SCM Frame" sheetId="9" r:id="rId8"/>
     <sheet name="Assignment01" sheetId="10" r:id="rId9"/>
     <sheet name="Assignment02" sheetId="12" r:id="rId10"/>
-    <sheet name="Ref." sheetId="3" r:id="rId11"/>
+    <sheet name="Assignment03" sheetId="13" r:id="rId11"/>
+    <sheet name="Ref." sheetId="3" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="135">
   <si>
     <t>Open</t>
     <phoneticPr fontId="1"/>
@@ -502,6 +503,12 @@
   </si>
   <si>
     <t>submite type</t>
+  </si>
+  <si>
+    <t>1) more suitable to use LIKE instead of =</t>
+  </si>
+  <si>
+    <t>fixed it. Used instead LIKE instead of "="</t>
   </si>
   <si>
     <t xml:space="preserve">fixed and added </t>
@@ -710,7 +717,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -792,6 +799,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -842,9 +855,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,6 +983,55 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>317501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>255679</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1250834</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21A6DB82-F51D-4CC2-B041-D5A2ACD56B01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6085417" y="740834"/>
+          <a:ext cx="3504762" cy="933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2793,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBB6DA5-C5EB-40B6-9E2E-F62F26A923B1}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:U4"/>
+    <sheetView view="pageBreakPreview" topLeftCell="J1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2829,30 +2888,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="17" t="s">
         <v>60</v>
       </c>
@@ -2879,27 +2938,27 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="28" t="s">
+      <c r="F2" s="40"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="44">
+      <c r="P2" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="28">
         <v>44207</v>
       </c>
       <c r="W2" s="18" t="s">
@@ -2923,29 +2982,29 @@
       <c r="E3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="28" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="40"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="42"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="44">
+      <c r="P3" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="28">
         <v>44207</v>
       </c>
       <c r="W3" s="18" t="s">
@@ -2969,29 +3028,29 @@
       <c r="E4" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="28" t="s">
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="40"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="42"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="44">
+      <c r="P4" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="28">
         <v>44207</v>
       </c>
       <c r="W4" s="18" t="s">
@@ -3019,24 +3078,12 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FFA9095A-E3FD-448E-9E33-BDAC5C3B1D29}">
           <x14:formula1>
             <xm:f>'Ref.'!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D5E55C52-C9D8-4551-8C33-AFD1B70A4727}">
-          <x14:formula1>
-            <xm:f>'Ref.'!$E$2:$E$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>W2:W4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C044DE1-8217-4519-B52C-0811E90EA5A8}">
-          <x14:formula1>
-            <xm:f>'Ref.'!$D$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>O2:O4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{772C9C2D-DC04-43BE-A110-9841097707D4}">
           <x14:formula1>
@@ -3057,6 +3104,175 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70C7B6F-17FC-476A-A336-4B7E8731F7B3}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" topLeftCell="G1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.5" style="15" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="15" customWidth="1"/>
+    <col min="6" max="14" width="9" style="15"/>
+    <col min="15" max="15" width="13" style="15" customWidth="1"/>
+    <col min="16" max="21" width="9" style="15"/>
+    <col min="22" max="22" width="14.625" style="15" customWidth="1"/>
+    <col min="23" max="23" width="12.5" style="15" customWidth="1"/>
+    <col min="24" max="24" width="32.5" style="15" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="33" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="123" customHeight="1">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20">
+        <v>44502</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="40"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="28">
+        <v>44238</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="X2" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="P2:U2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DCC0E4F8-EE92-462A-B436-8EACD4038C63}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AAFC3623-DABF-4384-80B4-BF832E0343B4}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$C$2:$C$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33D60C56-30A3-400F-A41B-2611068026A6}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$D$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C4BB7F41-B97A-4311-AB13-5F63AEE09F90}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$E$2:$E$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79D78B48-3EA6-4881-B010-C49ED03DA67C}">
+          <x14:formula1>
+            <xm:f>'Ref.'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -3251,7 +3467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="G4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="G4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
@@ -3287,30 +3503,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -3337,28 +3553,28 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>82</v>
       </c>
@@ -3383,28 +3599,28 @@
       <c r="E3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
       <c r="V3" s="18" t="s">
         <v>82</v>
       </c>
@@ -3429,28 +3645,28 @@
       <c r="E4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="31" t="s">
+      <c r="P4" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
       <c r="V4" s="18" t="s">
         <v>82</v>
       </c>
@@ -3521,7 +3737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13264516-45EC-4B12-9C49-DDC008555DF7}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="H4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="M4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
@@ -3557,30 +3773,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -3607,28 +3823,28 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>73</v>
       </c>
@@ -3653,28 +3869,28 @@
       <c r="E3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
       <c r="V3" s="18" t="s">
         <v>73</v>
       </c>
@@ -3699,28 +3915,28 @@
       <c r="E4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="31" t="s">
+      <c r="P4" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
       <c r="V4" s="18" t="s">
         <v>73</v>
       </c>
@@ -3790,7 +4006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5105948C-7804-4434-B607-79DA3F85CE6C}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="H1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="N1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
@@ -3826,30 +4042,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -3876,28 +4092,28 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>73</v>
       </c>
@@ -3962,7 +4178,7 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="M1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3997,30 +4213,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -4047,33 +4263,33 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>73</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="X2" s="18"/>
     </row>
@@ -4093,28 +4309,28 @@
       <c r="E3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
       <c r="V3" s="18" t="s">
         <v>73</v>
       </c>
@@ -4182,8 +4398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017E22DB-897C-4CBD-B355-A546CADAE648}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView view="pageBreakPreview" topLeftCell="S2" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4218,30 +4434,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -4268,26 +4484,26 @@
       <c r="E2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>66</v>
       </c>
@@ -4314,26 +4530,26 @@
       <c r="E3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
       <c r="V3" s="18" t="s">
         <v>66</v>
       </c>
@@ -4358,28 +4574,28 @@
       <c r="E4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="31" t="s">
+      <c r="P4" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
       <c r="V4" s="18" t="s">
         <v>66</v>
       </c>
@@ -4404,26 +4620,26 @@
       <c r="E5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28" t="s">
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="30"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
       <c r="V5" s="18" t="s">
         <v>66</v>
       </c>
@@ -4496,7 +4712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A935C436-83B6-4944-84D7-100E4F279E3B}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="L1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="G1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
@@ -4532,30 +4748,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="17" t="s">
         <v>60</v>
       </c>
@@ -4582,28 +4798,28 @@
       <c r="E2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>64</v>
       </c>
@@ -4667,7 +4883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79EE276-69FB-47B7-AEE4-B8429CEE434E}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J6" workbookViewId="0">
       <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
@@ -4703,30 +4919,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="17" t="s">
         <v>21</v>
       </c>
@@ -4753,33 +4969,33 @@
       <c r="E2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>86</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="X2" s="18"/>
     </row>
@@ -4799,31 +5015,31 @@
       <c r="E3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
       <c r="V3" s="18" t="s">
         <v>86</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="X3" s="18"/>
     </row>
@@ -4843,26 +5059,26 @@
       <c r="E4" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28" t="s">
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="31" t="s">
+      <c r="P4" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
       <c r="V4" s="18" t="s">
         <v>86</v>
       </c>
@@ -4887,26 +5103,26 @@
       <c r="E5" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28" t="s">
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="30"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
       <c r="V5" s="18" t="s">
         <v>86</v>
       </c>
@@ -4931,30 +5147,32 @@
       <c r="E6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28" t="s">
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
       <c r="V6" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="W6" s="18"/>
+      <c r="W6" s="18" t="s">
+        <v>124</v>
+      </c>
       <c r="X6" s="18"/>
     </row>
     <row r="7" spans="1:24" ht="252" customHeight="1">
@@ -4973,26 +5191,26 @@
       <c r="E7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28" t="s">
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="30"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="31" t="s">
+      <c r="P7" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
       <c r="V7" s="18" t="s">
         <v>86</v>
       </c>
@@ -5034,8 +5252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394B31C0-9FA0-4662-B312-DAF429ECDB72}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="L1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView view="pageBreakPreview" topLeftCell="O1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5070,30 +5288,30 @@
       <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="37"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="17" t="s">
         <v>60</v>
       </c>
@@ -5120,26 +5338,26 @@
       <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18" t="s">
         <v>64</v>
       </c>
@@ -5164,28 +5382,28 @@
       <c r="E3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
       <c r="V3" s="18" t="s">
         <v>64</v>
       </c>
@@ -5210,28 +5428,28 @@
       <c r="E4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="31" t="s">
+      <c r="P4" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
       <c r="V4" s="18" t="s">
         <v>64</v>
       </c>
@@ -5256,28 +5474,28 @@
       <c r="E5" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28" t="s">
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="30"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
       <c r="V5" s="18" t="s">
         <v>64</v>
       </c>
@@ -5302,28 +5520,28 @@
       <c r="E6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28" t="s">
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
       <c r="V6" s="18" t="s">
         <v>64</v>
       </c>
@@ -5348,28 +5566,28 @@
       <c r="E7" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28" t="s">
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="30"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="31" t="s">
+      <c r="P7" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
       <c r="V7" s="18" t="s">
         <v>64</v>
       </c>
@@ -5394,28 +5612,28 @@
       <c r="E8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28" t="s">
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="30"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="32"/>
       <c r="O8" s="16"/>
-      <c r="P8" s="31" t="s">
+      <c r="P8" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
       <c r="V8" s="18" t="s">
         <v>64</v>
       </c>
@@ -5440,26 +5658,26 @@
       <c r="E9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28" t="s">
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="32"/>
       <c r="O9" s="16"/>
-      <c r="P9" s="31" t="s">
+      <c r="P9" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
       <c r="V9" s="18" t="s">
         <v>64</v>
       </c>
@@ -5484,28 +5702,28 @@
       <c r="E10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28" t="s">
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="32"/>
       <c r="O10" s="16"/>
-      <c r="P10" s="31" t="s">
+      <c r="P10" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="33"/>
       <c r="V10" s="18" t="s">
         <v>64</v>
       </c>
@@ -5530,26 +5748,26 @@
       <c r="E11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28" t="s">
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="30"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="32"/>
       <c r="O11" s="16"/>
-      <c r="P11" s="31" t="s">
+      <c r="P11" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="31"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
       <c r="V11" s="18" t="s">
         <v>64</v>
       </c>
@@ -5599,18 +5817,12 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1B399EE9-1C37-4054-8D1B-EB08957349CA}">
           <x14:formula1>
             <xm:f>'Ref.'!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C11</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AFE683F6-95EC-486F-A8C6-7B798BFC7635}">
-          <x14:formula1>
-            <xm:f>'Ref.'!$E$2:$E$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>W2:W11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C621F27-68B6-4924-8123-0F05B771C401}">
           <x14:formula1>

</xml_diff>